<commit_message>
updated media composition and generated all draft reconstructions
</commit_message>
<xml_diff>
--- a/data/media_subsetted.xlsx
+++ b/data/media_subsetted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Documents/projects/go_pacm/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glm5uh/Documents/projects/go_pacm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94078D27-71D4-F742-8CA0-C1D1D7B308ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D98A7E3-ED2B-9B42-AB36-27DD36E8EBED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="0" windowWidth="12680" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="media_subsetted_with_catalog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="202">
   <si>
     <t>Class</t>
   </si>
@@ -488,12 +488,150 @@
   </si>
   <si>
     <t>Nitrilotriacetic acid</t>
+  </si>
+  <si>
+    <t>modelseed_id</t>
+  </si>
+  <si>
+    <t>cpd00027</t>
+  </si>
+  <si>
+    <t>cpd00082</t>
+  </si>
+  <si>
+    <t>cpd00158</t>
+  </si>
+  <si>
+    <t>cpd00179</t>
+  </si>
+  <si>
+    <t>cpd00208</t>
+  </si>
+  <si>
+    <t>cpd00003</t>
+  </si>
+  <si>
+    <t>cpd08053</t>
+  </si>
+  <si>
+    <t>cpd04145</t>
+  </si>
+  <si>
+    <t>cpd00984</t>
+  </si>
+  <si>
+    <t>cpd00205,cpd00099</t>
+  </si>
+  <si>
+    <t>cpd23056</t>
+  </si>
+  <si>
+    <t>flags_for_modeling</t>
+  </si>
+  <si>
+    <t>May have few reactions</t>
+  </si>
+  <si>
+    <t>cpd00119</t>
+  </si>
+  <si>
+    <t>cpd00322</t>
+  </si>
+  <si>
+    <t>cpd00107</t>
+  </si>
+  <si>
+    <t>cpd00060</t>
+  </si>
+  <si>
+    <t>cpd00156</t>
+  </si>
+  <si>
+    <t>cpd00051</t>
+  </si>
+  <si>
+    <t>cpd00084</t>
+  </si>
+  <si>
+    <t>cpd00023</t>
+  </si>
+  <si>
+    <t>cpd00066</t>
+  </si>
+  <si>
+    <t>cpd00129</t>
+  </si>
+  <si>
+    <t>cpd00132</t>
+  </si>
+  <si>
+    <t>cpd00041</t>
+  </si>
+  <si>
+    <t>cpd00053</t>
+  </si>
+  <si>
+    <t>cpd00054</t>
+  </si>
+  <si>
+    <t>cpd00161</t>
+  </si>
+  <si>
+    <t>cpd00035</t>
+  </si>
+  <si>
+    <t>cpd00033</t>
+  </si>
+  <si>
+    <t>cpd00039</t>
+  </si>
+  <si>
+    <t>cpd00065</t>
+  </si>
+  <si>
+    <t>cpd00069</t>
+  </si>
+  <si>
+    <t>cpd00128</t>
+  </si>
+  <si>
+    <t>cpd00207</t>
+  </si>
+  <si>
+    <t>cpd00092</t>
+  </si>
+  <si>
+    <t>cpd00309</t>
+  </si>
+  <si>
+    <t>cpd00205,cpd00029</t>
+  </si>
+  <si>
+    <t>cpd00048,cpd10515</t>
+  </si>
+  <si>
+    <t>cpd00254,cpd00099</t>
+  </si>
+  <si>
+    <t>cpd00048,cpd00034</t>
+  </si>
+  <si>
+    <t>cpd00149,cpd00209</t>
+  </si>
+  <si>
+    <t>cpd00048,cpd00205,cpd24344</t>
+  </si>
+  <si>
+    <t>cpd00971,cpd03387</t>
+  </si>
+  <si>
+    <t>cpd00971,cpd15574</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -971,8 +1109,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1327,16 +1466,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1352,8 +1491,14 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1372,8 +1517,11 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1392,8 +1540,11 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1412,8 +1563,11 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1432,8 +1586,11 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1452,8 +1609,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1472,8 +1632,11 @@
       <c r="F7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1492,8 +1655,11 @@
       <c r="F8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1512,8 +1678,11 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1532,8 +1701,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1552,8 +1724,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1572,8 +1747,14 @@
       <c r="F12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1592,8 +1773,11 @@
       <c r="F13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1612,8 +1796,11 @@
       <c r="F14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1632,8 +1819,11 @@
       <c r="F15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1652,8 +1842,11 @@
       <c r="F16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1672,8 +1865,11 @@
       <c r="F17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1692,8 +1888,11 @@
       <c r="F18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1712,8 +1911,11 @@
       <c r="F19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1732,8 +1934,11 @@
       <c r="F20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1752,8 +1957,11 @@
       <c r="F21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1772,8 +1980,11 @@
       <c r="F22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1792,8 +2003,11 @@
       <c r="F23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1812,8 +2026,11 @@
       <c r="F24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1832,8 +2049,11 @@
       <c r="F25" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1852,8 +2072,11 @@
       <c r="F26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1872,8 +2095,11 @@
       <c r="F27" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1892,8 +2118,11 @@
       <c r="F28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1912,8 +2141,11 @@
       <c r="F29" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1932,8 +2164,11 @@
       <c r="F30" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1952,8 +2187,11 @@
       <c r="F31" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
@@ -1972,8 +2210,11 @@
       <c r="F32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1992,8 +2233,11 @@
       <c r="F33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -2012,8 +2256,11 @@
       <c r="F34" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2032,8 +2279,11 @@
       <c r="F35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2052,8 +2302,11 @@
       <c r="F36" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -2072,8 +2325,11 @@
       <c r="F37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
@@ -2092,8 +2348,11 @@
       <c r="F38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2112,8 +2371,11 @@
       <c r="F39" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2132,8 +2394,11 @@
       <c r="F40" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>41</v>
       </c>
@@ -2152,8 +2417,11 @@
       <c r="F41" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>42</v>
       </c>
@@ -2172,8 +2440,11 @@
       <c r="F42" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>43</v>
       </c>
@@ -2192,8 +2463,11 @@
       <c r="F43" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>44</v>
       </c>
@@ -2212,8 +2486,11 @@
       <c r="F44" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2233,7 +2510,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2253,7 +2530,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2273,7 +2550,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>48</v>
       </c>

</xml_diff>